<commit_message>
{Update} architecture capsule 005, 006, 007, 008, 009, 012
</commit_message>
<xml_diff>
--- a/thématique SI/005 Décomposer le SI/conception/storyboard 005.xlsx
+++ b/thématique SI/005 Décomposer le SI/conception/storyboard 005.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10409"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26529"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/vincent/Library/Mobile Documents/com~apple~CloudDocs/Documents/pro/ISIS/2023-2024/dev/projet-FENS/thématique SI/005 Décomposer le SI/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Stage\projet-FENS\thématique SI\005 Décomposer le SI\conception\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{08856488-2061-5A48-B258-F2A7D55A041A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E944C94C-FC73-4D95-84A2-07B0C8C2D28E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5120" yWindow="840" windowWidth="35680" windowHeight="21000" xr2:uid="{A4F29CA4-E8D0-5846-A34B-CC524442BAF9}"/>
+    <workbookView xWindow="28680" yWindow="-15120" windowWidth="19440" windowHeight="15600" xr2:uid="{A4F29CA4-E8D0-5846-A34B-CC524442BAF9}"/>
   </bookViews>
   <sheets>
     <sheet name="E3-1-ISI1-4-005 SCEN" sheetId="8" r:id="rId1"/>
@@ -20,20 +20,12 @@
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
-    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
-      <xcalcf:calcFeatures>
-        <xcalcf:feature name="microsoft.com:RD"/>
-        <xcalcf:feature name="microsoft.com:FV"/>
-        <xcalcf:feature name="microsoft.com:LET_WF"/>
-        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
-      </xcalcf:calcFeatures>
-    </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="14" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Intéractions</t>
   </si>
@@ -78,6 +70,12 @@
   </si>
   <si>
     <t>Capacités visées</t>
+  </si>
+  <si>
+    <t>c010</t>
+  </si>
+  <si>
+    <t>Decomposer le SI</t>
   </si>
 </sst>
 </file>
@@ -138,9 +136,6 @@
   </cellStyleXfs>
   <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -156,6 +151,9 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -178,16 +176,16 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>1</xdr:col>
+      <xdr:col>2</xdr:col>
       <xdr:colOff>92031</xdr:colOff>
       <xdr:row>5</xdr:row>
       <xdr:rowOff>105653</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>1688733</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>1692543</xdr:colOff>
       <xdr:row>5</xdr:row>
-      <xdr:rowOff>1885647</xdr:rowOff>
+      <xdr:rowOff>1889457</xdr:rowOff>
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
@@ -222,14 +220,14 @@
   </xdr:twoCellAnchor>
   <xdr:twoCellAnchor editAs="oneCell">
     <xdr:from>
-      <xdr:col>2</xdr:col>
+      <xdr:col>3</xdr:col>
       <xdr:colOff>151081</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>131908</xdr:rowOff>
     </xdr:from>
     <xdr:to>
-      <xdr:col>2</xdr:col>
-      <xdr:colOff>4210327</xdr:colOff>
+      <xdr:col>3</xdr:col>
+      <xdr:colOff>4206517</xdr:colOff>
       <xdr:row>8</xdr:row>
       <xdr:rowOff>2438528</xdr:rowOff>
     </xdr:to>
@@ -564,78 +562,84 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EF2AF475-8297-9B48-A5BF-C8EFBB80C1A0}">
-  <dimension ref="A1:E9"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="184" zoomScaleNormal="184" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="C9" sqref="C9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="17.83203125" customWidth="1"/>
-    <col min="2" max="2" width="17.6640625" customWidth="1"/>
-    <col min="3" max="3" width="58.1640625" customWidth="1"/>
-    <col min="4" max="4" width="53.33203125" style="3" customWidth="1"/>
-    <col min="5" max="6" width="26.6640625" customWidth="1"/>
+    <col min="1" max="1" width="11.19921875" style="7"/>
+    <col min="2" max="2" width="17.796875" customWidth="1"/>
+    <col min="3" max="3" width="17.69921875" customWidth="1"/>
+    <col min="4" max="4" width="58.19921875" customWidth="1"/>
+    <col min="5" max="5" width="53.296875" style="2" customWidth="1"/>
+    <col min="6" max="7" width="26.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A1" s="6" t="s">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B1" s="5" t="s">
         <v>7</v>
       </c>
-      <c r="B1" t="s">
+      <c r="C1" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A2" s="6" t="s">
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B2" s="5" t="s">
         <v>9</v>
       </c>
-      <c r="B2" t="s">
+      <c r="C2" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A3" s="2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B3" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A4" s="2" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="B4" s="7"/>
-    </row>
-    <row r="6" spans="1:5" ht="154" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="2" t="s">
+      <c r="C4" s="6"/>
+    </row>
+    <row r="6" spans="1:6" ht="154.05000000000001" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B6" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="7" spans="1:5" ht="41" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="2" t="s">
+    <row r="7" spans="1:6" ht="40.950000000000003" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B7" s="1" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
-      <c r="A8" s="2" t="s">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="B8" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="B8" s="2" t="s">
+      <c r="C8" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="D8" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="D8" s="4" t="s">
+      <c r="E8" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="E8" s="2" t="s">
+      <c r="F8" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="9" spans="1:5" ht="201" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B9" s="1"/>
-      <c r="D9" s="5" t="s">
+    <row r="9" spans="1:6" ht="201" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="7" t="s">
+        <v>13</v>
+      </c>
+      <c r="C9" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="4" t="s">
         <v>6</v>
       </c>
     </row>

</xml_diff>